<commit_message>
add other cities estimates and near final
</commit_message>
<xml_diff>
--- a/output/California_ACS_Population.xlsx
+++ b/output/California_ACS_Population.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5185207C-C584-46EA-B3E8-867F1021FDAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F21D1-C0E0-447C-9A32-F5EA88930231}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:P44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:G38"/>
+      <selection activeCell="K43" sqref="K43:P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,8 +1387,1022 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>599414</v>
+      </c>
+      <c r="C6">
+        <v>56.73</v>
+      </c>
+      <c r="D6">
+        <v>56.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>263940</v>
+      </c>
+      <c r="C7">
+        <v>24.98</v>
+      </c>
+      <c r="D7">
+        <v>81.709999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>193229</v>
+      </c>
+      <c r="C8">
+        <v>18.29</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1056583</v>
+      </c>
+      <c r="C10" s="3">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>495758</v>
+      </c>
+      <c r="C15">
+        <v>46.92</v>
+      </c>
+      <c r="D15">
+        <v>46.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>560825</v>
+      </c>
+      <c r="C16">
+        <v>53.08</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1056583</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4101</v>
+      </c>
+      <c r="C23">
+        <v>0.39</v>
+      </c>
+      <c r="D23">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1">
+        <v>451416</v>
+      </c>
+      <c r="C24">
+        <v>42.72</v>
+      </c>
+      <c r="D24">
+        <v>43.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>83473</v>
+      </c>
+      <c r="C25">
+        <v>7.9</v>
+      </c>
+      <c r="D25">
+        <v>51.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1">
+        <v>365242</v>
+      </c>
+      <c r="C26">
+        <v>34.57</v>
+      </c>
+      <c r="D26">
+        <v>85.58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>97326</v>
+      </c>
+      <c r="C27">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="D27">
+        <v>94.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1">
+        <v>55025</v>
+      </c>
+      <c r="C28">
+        <v>5.21</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1056583</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="e">
+        <f>- female</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3370</v>
+      </c>
+      <c r="C39" s="1">
+        <v>258</v>
+      </c>
+      <c r="D39" s="1">
+        <v>5</v>
+      </c>
+      <c r="E39" s="1">
+        <v>438</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="1">
+        <v>210911</v>
+      </c>
+      <c r="C40" s="1">
+        <v>8412</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1032</v>
+      </c>
+      <c r="E40" s="1">
+        <v>221743</v>
+      </c>
+      <c r="F40" s="1">
+        <v>7737</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1">
+        <v>37099</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1">
+        <v>46374</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="1">
+        <v>7550</v>
+      </c>
+      <c r="C42" s="1">
+        <v>93097</v>
+      </c>
+      <c r="D42" s="1">
+        <v>63081</v>
+      </c>
+      <c r="E42" s="1">
+        <v>8342</v>
+      </c>
+      <c r="F42" s="1">
+        <v>108134</v>
+      </c>
+      <c r="G42" s="1">
+        <v>85038</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1">
+        <v>7483</v>
+      </c>
+      <c r="C43" s="1">
+        <v>19325</v>
+      </c>
+      <c r="D43" s="1">
+        <v>15309</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6743</v>
+      </c>
+      <c r="F43" s="1">
+        <v>22834</v>
+      </c>
+      <c r="G43" s="1">
+        <v>25632</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1">
+        <v>26329</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1918</v>
+      </c>
+      <c r="D44">
+        <v>579</v>
+      </c>
+      <c r="E44" s="1">
+        <v>23032</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2225</v>
+      </c>
+      <c r="G44">
+        <v>942</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034F0695-5F85-449A-AF56-7D70892D28D5}">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>285651</v>
+      </c>
+      <c r="C6">
+        <v>57.67</v>
+      </c>
+      <c r="D6">
+        <v>57.67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>123959</v>
+      </c>
+      <c r="C7">
+        <v>25.03</v>
+      </c>
+      <c r="D7">
+        <v>82.69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>85717</v>
+      </c>
+      <c r="C8">
+        <v>17.309999999999999</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <v>495327</v>
+      </c>
+      <c r="C10" s="3">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1">
+        <v>226804</v>
+      </c>
+      <c r="C15">
+        <v>45.79</v>
+      </c>
+      <c r="D15">
+        <v>45.79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>268523</v>
+      </c>
+      <c r="C16">
+        <v>54.21</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>495327</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1624</v>
+      </c>
+      <c r="C23">
+        <v>0.33</v>
+      </c>
+      <c r="D23">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1">
+        <v>205505</v>
+      </c>
+      <c r="C24">
+        <v>41.49</v>
+      </c>
+      <c r="D24">
+        <v>41.82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>51096</v>
+      </c>
+      <c r="C25">
+        <v>10.32</v>
+      </c>
+      <c r="D25">
+        <v>52.13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1">
+        <v>165350</v>
+      </c>
+      <c r="C26">
+        <v>33.380000000000003</v>
+      </c>
+      <c r="D26">
+        <v>85.51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>56186</v>
+      </c>
+      <c r="C27">
+        <v>11.34</v>
+      </c>
+      <c r="D27">
+        <v>96.86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1">
+        <v>15566</v>
+      </c>
+      <c r="C28">
+        <v>3.14</v>
+      </c>
+      <c r="D28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1">
+        <v>495327</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="e">
+        <f>- female</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1237</v>
+      </c>
+      <c r="C39" s="1">
+        <v>115</v>
+      </c>
+      <c r="D39" s="1">
+        <v>19</v>
+      </c>
+      <c r="E39" s="1">
+        <v>253</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="1">
+        <v>92071</v>
+      </c>
+      <c r="C40" s="1">
+        <v>3928</v>
+      </c>
+      <c r="D40">
+        <v>670</v>
+      </c>
+      <c r="E40" s="1">
+        <v>103605</v>
+      </c>
+      <c r="F40" s="1">
+        <v>3875</v>
+      </c>
+      <c r="G40" s="1">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="1">
+        <v>23586</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1">
+        <v>27510</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="1">
+        <v>5066</v>
+      </c>
+      <c r="C42" s="1">
+        <v>41427</v>
+      </c>
+      <c r="D42" s="1">
+        <v>25615</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5426</v>
+      </c>
+      <c r="F42" s="1">
+        <v>50032</v>
+      </c>
+      <c r="G42" s="1">
+        <v>37784</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1">
+        <v>5766</v>
+      </c>
+      <c r="C43" s="1">
+        <v>10467</v>
+      </c>
+      <c r="D43" s="1">
+        <v>7856</v>
+      </c>
+      <c r="E43" s="1">
+        <v>7043</v>
+      </c>
+      <c r="F43" s="1">
+        <v>13141</v>
+      </c>
+      <c r="G43" s="1">
+        <v>11913</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1">
+        <v>8546</v>
+      </c>
+      <c r="C44">
+        <v>272</v>
+      </c>
+      <c r="D44">
+        <v>163</v>
+      </c>
+      <c r="E44" s="1">
+        <v>5542</v>
+      </c>
+      <c r="F44">
+        <v>702</v>
+      </c>
+      <c r="G44">
+        <v>341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A709906B-ABD6-4266-899E-4F436CA69F2B}">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,1019 +2432,6 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>599414</v>
-      </c>
-      <c r="C6">
-        <v>56.73</v>
-      </c>
-      <c r="D6">
-        <v>56.73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>263940</v>
-      </c>
-      <c r="C7">
-        <v>24.98</v>
-      </c>
-      <c r="D7">
-        <v>81.709999999999994</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>193229</v>
-      </c>
-      <c r="C8">
-        <v>18.29</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
-        <v>1056583</v>
-      </c>
-      <c r="C10" s="3">
-        <v>100</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>495758</v>
-      </c>
-      <c r="C15">
-        <v>46.92</v>
-      </c>
-      <c r="D15">
-        <v>46.92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>560825</v>
-      </c>
-      <c r="C16">
-        <v>53.08</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1">
-        <v>1056583</v>
-      </c>
-      <c r="C18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1">
-        <v>4101</v>
-      </c>
-      <c r="C23">
-        <v>0.39</v>
-      </c>
-      <c r="D23">
-        <v>0.39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1">
-        <v>451416</v>
-      </c>
-      <c r="C24">
-        <v>42.72</v>
-      </c>
-      <c r="D24">
-        <v>43.11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1">
-        <v>83473</v>
-      </c>
-      <c r="C25">
-        <v>7.9</v>
-      </c>
-      <c r="D25">
-        <v>51.01</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="1">
-        <v>365242</v>
-      </c>
-      <c r="C26">
-        <v>34.57</v>
-      </c>
-      <c r="D26">
-        <v>85.58</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="1">
-        <v>97326</v>
-      </c>
-      <c r="C27">
-        <v>9.2100000000000009</v>
-      </c>
-      <c r="D27">
-        <v>94.79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="1">
-        <v>55025</v>
-      </c>
-      <c r="C28">
-        <v>5.21</v>
-      </c>
-      <c r="D28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="1">
-        <v>1056583</v>
-      </c>
-      <c r="C30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" t="e">
-        <f>- female</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="1">
-        <v>3370</v>
-      </c>
-      <c r="C39" s="1">
-        <v>258</v>
-      </c>
-      <c r="D39" s="1">
-        <v>5</v>
-      </c>
-      <c r="E39" s="1">
-        <v>438</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="1">
-        <v>210911</v>
-      </c>
-      <c r="C40" s="1">
-        <v>8412</v>
-      </c>
-      <c r="D40" s="1">
-        <v>1032</v>
-      </c>
-      <c r="E40" s="1">
-        <v>221743</v>
-      </c>
-      <c r="F40" s="1">
-        <v>7737</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="1">
-        <v>37099</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1">
-        <v>46374</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="1">
-        <v>7550</v>
-      </c>
-      <c r="C42" s="1">
-        <v>93097</v>
-      </c>
-      <c r="D42" s="1">
-        <v>63081</v>
-      </c>
-      <c r="E42" s="1">
-        <v>8342</v>
-      </c>
-      <c r="F42" s="1">
-        <v>108134</v>
-      </c>
-      <c r="G42" s="1">
-        <v>85038</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="1">
-        <v>7483</v>
-      </c>
-      <c r="C43" s="1">
-        <v>19325</v>
-      </c>
-      <c r="D43" s="1">
-        <v>15309</v>
-      </c>
-      <c r="E43" s="1">
-        <v>6743</v>
-      </c>
-      <c r="F43" s="1">
-        <v>22834</v>
-      </c>
-      <c r="G43" s="1">
-        <v>25632</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="1">
-        <v>26329</v>
-      </c>
-      <c r="C44" s="1">
-        <v>1918</v>
-      </c>
-      <c r="D44">
-        <v>579</v>
-      </c>
-      <c r="E44" s="1">
-        <v>23032</v>
-      </c>
-      <c r="F44" s="1">
-        <v>2225</v>
-      </c>
-      <c r="G44">
-        <v>942</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034F0695-5F85-449A-AF56-7D70892D28D5}">
-  <dimension ref="A1:I44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>285651</v>
-      </c>
-      <c r="C6">
-        <v>57.67</v>
-      </c>
-      <c r="D6">
-        <v>57.67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>123959</v>
-      </c>
-      <c r="C7">
-        <v>25.03</v>
-      </c>
-      <c r="D7">
-        <v>82.69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>85717</v>
-      </c>
-      <c r="C8">
-        <v>17.309999999999999</v>
-      </c>
-      <c r="D8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4">
-        <v>495327</v>
-      </c>
-      <c r="C10" s="3">
-        <v>100</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>226804</v>
-      </c>
-      <c r="C15">
-        <v>45.79</v>
-      </c>
-      <c r="D15">
-        <v>45.79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
-        <v>268523</v>
-      </c>
-      <c r="C16">
-        <v>54.21</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="1">
-        <v>495327</v>
-      </c>
-      <c r="C18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="1">
-        <v>1624</v>
-      </c>
-      <c r="C23">
-        <v>0.33</v>
-      </c>
-      <c r="D23">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1">
-        <v>205505</v>
-      </c>
-      <c r="C24">
-        <v>41.49</v>
-      </c>
-      <c r="D24">
-        <v>41.82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1">
-        <v>51096</v>
-      </c>
-      <c r="C25">
-        <v>10.32</v>
-      </c>
-      <c r="D25">
-        <v>52.13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="1">
-        <v>165350</v>
-      </c>
-      <c r="C26">
-        <v>33.380000000000003</v>
-      </c>
-      <c r="D26">
-        <v>85.51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="1">
-        <v>56186</v>
-      </c>
-      <c r="C27">
-        <v>11.34</v>
-      </c>
-      <c r="D27">
-        <v>96.86</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="1">
-        <v>15566</v>
-      </c>
-      <c r="C28">
-        <v>3.14</v>
-      </c>
-      <c r="D28">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="1">
-        <v>495327</v>
-      </c>
-      <c r="C30">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F36" t="e">
-        <f>- female</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1237</v>
-      </c>
-      <c r="C39" s="1">
-        <v>115</v>
-      </c>
-      <c r="D39" s="1">
-        <v>19</v>
-      </c>
-      <c r="E39" s="1">
-        <v>253</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="1">
-        <v>92071</v>
-      </c>
-      <c r="C40" s="1">
-        <v>3928</v>
-      </c>
-      <c r="D40">
-        <v>670</v>
-      </c>
-      <c r="E40" s="1">
-        <v>103605</v>
-      </c>
-      <c r="F40" s="1">
-        <v>3875</v>
-      </c>
-      <c r="G40" s="1">
-        <v>1356</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="1">
-        <v>23586</v>
-      </c>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1">
-        <v>27510</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>21</v>
-      </c>
-      <c r="B42" s="1">
-        <v>5066</v>
-      </c>
-      <c r="C42" s="1">
-        <v>41427</v>
-      </c>
-      <c r="D42" s="1">
-        <v>25615</v>
-      </c>
-      <c r="E42" s="1">
-        <v>5426</v>
-      </c>
-      <c r="F42" s="1">
-        <v>50032</v>
-      </c>
-      <c r="G42" s="1">
-        <v>37784</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="1">
-        <v>5766</v>
-      </c>
-      <c r="C43" s="1">
-        <v>10467</v>
-      </c>
-      <c r="D43" s="1">
-        <v>7856</v>
-      </c>
-      <c r="E43" s="1">
-        <v>7043</v>
-      </c>
-      <c r="F43" s="1">
-        <v>13141</v>
-      </c>
-      <c r="G43" s="1">
-        <v>11913</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="1">
-        <v>8546</v>
-      </c>
-      <c r="C44">
-        <v>272</v>
-      </c>
-      <c r="D44">
-        <v>163</v>
-      </c>
-      <c r="E44" s="1">
-        <v>5542</v>
-      </c>
-      <c r="F44">
-        <v>702</v>
-      </c>
-      <c r="G44">
-        <v>341</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A709906B-ABD6-4266-899E-4F436CA69F2B}">
-  <dimension ref="A1:I44"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -2905,12 +2906,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDDD9FE7-4B28-4AC9-AF11-4BC69F24F245}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>